<commit_message>
class and access level
</commit_message>
<xml_diff>
--- a/Swift To Kotlin.xlsx
+++ b/Swift To Kotlin.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palashroy/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FDD760-921D-0D46-823C-813BCE8F04B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85734B9A-06D2-C94D-8AD6-34688621B2A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{523F9392-1A58-6441-802E-A371D117E942}"/>
+    <workbookView xWindow="-43680" yWindow="-3580" windowWidth="37660" windowHeight="21400" activeTab="2" xr2:uid="{523F9392-1A58-6441-802E-A371D117E942}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
     <sheet name="Func" sheetId="2" r:id="rId2"/>
+    <sheet name="Class" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="199">
   <si>
     <t>Swift Syntax</t>
   </si>
@@ -697,6 +698,73 @@
     <t>var temperature = 10
 var message = "The water temperature is \(temperature &gt; 50 ?   "Too Hot" :  "Cold")."
 print(message)</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>class Cars {
+    var color =  "Blue"
+    var transmission = "Manual"
+    var model = "Honda"
+    var make = 2021
+}</t>
+  </si>
+  <si>
+    <t>NO diff
+In Kotlin, we create a function that would call cars and that function will be called from Main.kt main method.</t>
+  </si>
+  <si>
+    <t>constructor</t>
+  </si>
+  <si>
+    <t>constructor is completely different in swift and Kotlin. Swift needs to declare init() to provide parameter, but kotclin class can have construtor in its declaration as shown in the example.</t>
+  </si>
+  <si>
+    <t>class Cars(var color: String, var maxSpeed: Int) {
+    var transmission = "Manual"
+    var model = "Honda"
+    var make = 2021
+    var details = ""
+    init {
+       details = "This is a $color $make $model with a $transmission transmission and $maxSpeed as max speed"
+    }
+}</t>
+  </si>
+  <si>
+    <t>class Car {
+    var transmission = "Manual"
+    var model = "Honda"
+    var make = 2021
+    var color: String
+    var maxSpeed: Int
+    var details: String
+    init(color: String, maxSpeed: Int){
+        self.color = color
+        self.maxSpeed = maxSpeed
+        details = "This is a \(color) \(make) \(model) with a \(transmission) transmission and \(maxSpeed) as max speed"
+    }
+}</t>
+  </si>
+  <si>
+    <t>visibility 
+modifiers</t>
+  </si>
+  <si>
+    <t>private : Limited to only class
+file-private: Limited to file, not just the class.
+Internal: Limited to framework or file.
+Open: Open to whole application. 
+Public: Public is same as open but not accessibkle outside module.</t>
+  </si>
+  <si>
+    <t>private: Limited to class only 
+protected: Same as Private, but visible to subclasses
+internal: Visile to module/library.
+Public: Visible all the way, inside and outside of the class and Module</t>
+  </si>
+  <si>
+    <t>In Swift we have 5 modifiers and in Kotlin 4. By default in swift is internal, but in Kotlin the default access level is Public</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1263,7 @@
   <sheetViews>
     <sheetView zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2401,9 +2469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC483575-FEAE-114C-89A9-2586A59B45AA}">
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4:E4"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3487,4 +3555,516 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F8EADC-7B3C-5C48-96EF-ADD84447D5AB}">
+  <dimension ref="A1:N46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4:M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="31" customFormat="1" ht="27">
+      <c r="A1" s="28"/>
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+    </row>
+    <row r="2" spans="1:14" ht="96" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+    </row>
+    <row r="3" spans="1:14" ht="289" customHeight="1">
+      <c r="A3" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="1:14" ht="107" customHeight="1">
+      <c r="A4" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" s="10"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" s="10"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" s="10"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="B8" s="10"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" s="10"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" s="10"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="B12" s="10"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14" s="10"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15" s="10"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="10"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="10"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="10"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="10"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="10"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="10"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="10"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="10"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="10"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="10"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="10"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="10"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="10"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="10"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="12"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="10"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="10"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="12"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="10"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="10"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="10"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="12"/>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="J2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>